<commit_message>
Further changes to the config inputs file to ensure that the newest assumption values are carried into the model.
</commit_message>
<xml_diff>
--- a/data/config_inputs/lhc_config_inputs_v5.xlsx
+++ b/data/config_inputs/lhc_config_inputs_v5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csucloudservices-my.sharepoint.com/personal/elliot_royle_mlcsu_nhs_uk/Documents/Git/Lung Health Checks/data/config_inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{DEB216A3-46EC-4ECC-9D1E-00EE1BB3E5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54BBC27C-C087-4905-A554-CE62BFE12D48}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{DEB216A3-46EC-4ECC-9D1E-00EE1BB3E5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8441074-3450-4F1D-983E-93EBB26C4282}"/>
   <bookViews>
-    <workbookView xWindow="28200" yWindow="0" windowWidth="28230" windowHeight="16200" activeTab="8" xr2:uid="{EEFCE178-3DE7-40FB-BEDD-2901AD1232AA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28200" windowHeight="16200" activeTab="8" xr2:uid="{EEFCE178-3DE7-40FB-BEDD-2901AD1232AA}"/>
   </bookViews>
   <sheets>
     <sheet name="frontpage" sheetId="1" r:id="rId1"/>
@@ -6734,7 +6734,9 @@
   </sheetPr>
   <dimension ref="B2:I16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16:I16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6910,19 +6912,19 @@
         <v>8</v>
       </c>
       <c r="E8" s="10">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="F8" s="10">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="G8" s="10">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="H8" s="10">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="I8" s="10">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Amendments to the assumptions config workbook to ensure M24 FU assumption is placed before the M3 cancer rate due to chronology.
</commit_message>
<xml_diff>
--- a/data/config_inputs/lhc_config_inputs_v5.xlsx
+++ b/data/config_inputs/lhc_config_inputs_v5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csucloudservices-my.sharepoint.com/personal/elliot_royle_mlcsu_nhs_uk/Documents/Git/Lung Health Checks/data/config_inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{DEB216A3-46EC-4ECC-9D1E-00EE1BB3E5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8441074-3450-4F1D-983E-93EBB26C4282}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="8_{DEB216A3-46EC-4ECC-9D1E-00EE1BB3E5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EEFD45B-4BC4-41E8-9A57-4600F4BD406D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28200" windowHeight="16200" activeTab="8" xr2:uid="{EEFCE178-3DE7-40FB-BEDD-2901AD1232AA}"/>
+    <workbookView xWindow="28215" yWindow="0" windowWidth="28215" windowHeight="16200" activeTab="8" xr2:uid="{EEFCE178-3DE7-40FB-BEDD-2901AD1232AA}"/>
   </bookViews>
   <sheets>
     <sheet name="frontpage" sheetId="1" r:id="rId1"/>
@@ -1078,7 +1078,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1114,6 +1114,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6734,9 +6735,7 @@
   </sheetPr>
   <dimension ref="B2:I16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16:I16"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6877,54 +6876,54 @@
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>75</v>
+        <v>283</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>35</v>
+        <v>284</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="10">
-        <v>0.8</v>
+        <v>0.25</v>
       </c>
       <c r="F7" s="10">
-        <v>0.8</v>
+        <v>0.25</v>
       </c>
       <c r="G7" s="10">
-        <v>0.8</v>
+        <v>0.25</v>
       </c>
       <c r="H7" s="10">
-        <v>0.8</v>
+        <v>0.25</v>
       </c>
       <c r="I7" s="10">
-        <v>0.8</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>283</v>
+        <v>75</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>284</v>
+        <v>35</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="10">
-        <v>0.25</v>
+        <v>0.8</v>
       </c>
       <c r="F8" s="10">
-        <v>0.25</v>
+        <v>0.8</v>
       </c>
       <c r="G8" s="10">
-        <v>0.25</v>
+        <v>0.8</v>
       </c>
       <c r="H8" s="10">
-        <v>0.25</v>
+        <v>0.8</v>
       </c>
       <c r="I8" s="10">
-        <v>0.25</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
@@ -7119,32 +7118,32 @@
       <c r="D16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="19">
+      <c r="E16" s="20">
         <f>1-SUM(E9:E15)</f>
         <v>6.3000000000000056E-2</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F16" s="20">
         <f t="shared" ref="F16:I16" si="0">1-SUM(F9:F15)</f>
         <v>6.3000000000000056E-2</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="20">
         <f t="shared" si="0"/>
         <v>6.3000000000000056E-2</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="20">
         <f t="shared" si="0"/>
         <v>6.3000000000000056E-2</v>
       </c>
-      <c r="I16" s="19">
+      <c r="I16" s="20">
         <f t="shared" si="0"/>
         <v>6.3000000000000056E-2</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="6V24wSd5WX1YfE+kEJw8LDeG/ApBKDpCZmLdhwnh6gakYy91ZFgU0nz59xO+WNYdJ7ZlhYsGSrstlDhxz/FCog==" saltValue="DFBPRPREa9WAe+QBpMxquw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="oGJcuUE0Zm+qk14ioL0wJ+0VJW30CBmrJogXXt9slWm+wfTDd20WdpooWQk8loOIRE2J5yPcDfc4ssWGTgvayA==" saltValue="mqRDyZKsbtsdhQ9wgOpjdg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <phoneticPr fontId="7" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:I16" xr:uid="{5E73C5F2-0875-4E9B-941B-B7E9ED0E7EE2}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9:I16 E3:I8" xr:uid="{5E73C5F2-0875-4E9B-941B-B7E9ED0E7EE2}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Updating of the V5 config input workbook inline with removal of bone abnormalities incidental.
</commit_message>
<xml_diff>
--- a/data/config_inputs/lhc_config_inputs_v5.xlsx
+++ b/data/config_inputs/lhc_config_inputs_v5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csucloudservices-my.sharepoint.com/personal/elliot_royle_mlcsu_nhs_uk/Documents/Git/Lung Health Checks/data/config_inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="8_{DEB216A3-46EC-4ECC-9D1E-00EE1BB3E5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EEFD45B-4BC4-41E8-9A57-4600F4BD406D}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{DEB216A3-46EC-4ECC-9D1E-00EE1BB3E5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1977D35A-792E-4C23-926B-F32D2B4F4A27}"/>
   <bookViews>
-    <workbookView xWindow="28215" yWindow="0" windowWidth="28215" windowHeight="16200" activeTab="8" xr2:uid="{EEFCE178-3DE7-40FB-BEDD-2901AD1232AA}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="29010" windowHeight="15585" firstSheet="7" activeTab="15" xr2:uid="{EEFCE178-3DE7-40FB-BEDD-2901AD1232AA}"/>
   </bookViews>
   <sheets>
     <sheet name="frontpage" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="280">
   <si>
     <t>Target Lung Health Check Modelling - Model Inputs</t>
   </si>
@@ -655,9 +655,6 @@
     <t>Percentage of Patients with Consolidation</t>
   </si>
   <si>
-    <t>Percentage of Patients with Bone abnormalities</t>
-  </si>
-  <si>
     <t>Percentage of Patients with Fractures with no trauma history</t>
   </si>
   <si>
@@ -718,9 +715,6 @@
     <t>init_inc_con</t>
   </si>
   <si>
-    <t>init_inc_bon</t>
-  </si>
-  <si>
     <t>init_inc_fra</t>
   </si>
   <si>
@@ -781,9 +775,6 @@
     <t>m3_inc_con</t>
   </si>
   <si>
-    <t>m3_inc_bon</t>
-  </si>
-  <si>
     <t>m3_inc_fra</t>
   </si>
   <si>
@@ -844,9 +835,6 @@
     <t>m12_inc_con</t>
   </si>
   <si>
-    <t>m12_inc_bon</t>
-  </si>
-  <si>
     <t>m12_inc_fra</t>
   </si>
   <si>
@@ -905,9 +893,6 @@
   </si>
   <si>
     <t>m24_inc_con</t>
-  </si>
-  <si>
-    <t>m24_inc_bon</t>
   </si>
   <si>
     <t>m24_inc_fra</t>
@@ -1078,7 +1063,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1114,7 +1099,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1695,10 +1679,10 @@
   <sheetPr codeName="Sheet10">
     <tabColor rgb="FFFFF2CC"/>
   </sheetPr>
-  <dimension ref="B2:I23"/>
+  <dimension ref="B2:I22"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1736,10 +1720,10 @@
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -1762,7 +1746,7 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>175</v>
@@ -1788,7 +1772,7 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>176</v>
@@ -1814,7 +1798,7 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>177</v>
@@ -1840,7 +1824,7 @@
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>178</v>
@@ -1866,7 +1850,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>179</v>
@@ -1892,7 +1876,7 @@
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>180</v>
@@ -1918,7 +1902,7 @@
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>181</v>
@@ -1944,7 +1928,7 @@
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>182</v>
@@ -1970,7 +1954,7 @@
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>183</v>
@@ -1996,7 +1980,7 @@
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>184</v>
@@ -2022,7 +2006,7 @@
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>185</v>
@@ -2048,7 +2032,7 @@
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>186</v>
@@ -2074,7 +2058,7 @@
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>187</v>
@@ -2100,10 +2084,10 @@
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
@@ -2126,7 +2110,7 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>188</v>
@@ -2152,7 +2136,7 @@
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>189</v>
@@ -2161,24 +2145,24 @@
         <v>8</v>
       </c>
       <c r="E19" s="10">
-        <v>2.3966446974236066E-3</v>
+        <v>1.1983223487118033E-3</v>
       </c>
       <c r="F19" s="10">
-        <v>2.3966446974236066E-3</v>
+        <v>1.1983223487118033E-3</v>
       </c>
       <c r="G19" s="10">
-        <v>2.3966446974236066E-3</v>
+        <v>1.1983223487118033E-3</v>
       </c>
       <c r="H19" s="10">
-        <v>2.3966446974236066E-3</v>
+        <v>1.1983223487118033E-3</v>
       </c>
       <c r="I19" s="10">
-        <v>2.3966446974236066E-3</v>
+        <v>1.1983223487118033E-3</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>190</v>
@@ -2204,7 +2188,7 @@
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>191</v>
@@ -2230,7 +2214,7 @@
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>192</v>
@@ -2238,53 +2222,26 @@
       <c r="D22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="10">
-        <v>1.1983223487118033E-3</v>
-      </c>
-      <c r="F22" s="10">
-        <v>1.1983223487118033E-3</v>
-      </c>
-      <c r="G22" s="10">
-        <v>1.1983223487118033E-3</v>
-      </c>
-      <c r="H22" s="10">
-        <v>1.1983223487118033E-3</v>
-      </c>
-      <c r="I22" s="10">
-        <v>1.1983223487118033E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="4">
-        <f>1-SUM(E3:E22)</f>
-        <v>5.9916117435609983E-4</v>
-      </c>
-      <c r="F23" s="4">
-        <v>5.9916117435590164E-4</v>
-      </c>
-      <c r="G23" s="4">
-        <v>5.9916117435590164E-4</v>
-      </c>
-      <c r="H23" s="4">
-        <v>5.9916117435590164E-4</v>
-      </c>
-      <c r="I23" s="4">
-        <v>5.9916117435590164E-4</v>
+      <c r="E22" s="19">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="F22" s="19">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="G22" s="19">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="H22" s="19">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="I22" s="19">
+        <v>5.9999999999999995E-4</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="8d/O1WlMpRKhAtu9jLjnI5iTtgf8mxB79zXrdukzdXX26FM3f5j3PoLOtfy2/hsvcsqUOkvTBybwO/RbSYbNrg==" saltValue="nM9vWrTJyGwsOA7+h+pEpg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="1+hkOEMOzNw0tEMYAtVoi4F9XM/W3HV3PIlcM9Oj0YjOkM++AYKe7fnVsdfMvG73GlRiyZi4JvM/tberEecYeQ==" saltValue="BmoLlpqCpN+SMl0VQ5k9RQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:I23" xr:uid="{C2D4DCCC-2F6E-43B5-9BE7-2CCD33112B93}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:I22" xr:uid="{C2D4DCCC-2F6E-43B5-9BE7-2CCD33112B93}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -2935,10 +2892,10 @@
   <sheetPr codeName="Sheet13">
     <tabColor rgb="FFFFF2CC"/>
   </sheetPr>
-  <dimension ref="B2:I23"/>
+  <dimension ref="B2:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2976,10 +2933,10 @@
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -3002,7 +2959,7 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>175</v>
@@ -3028,7 +2985,7 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>176</v>
@@ -3054,7 +3011,7 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>177</v>
@@ -3080,7 +3037,7 @@
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>178</v>
@@ -3106,7 +3063,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>179</v>
@@ -3132,7 +3089,7 @@
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>180</v>
@@ -3158,7 +3115,7 @@
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>181</v>
@@ -3184,7 +3141,7 @@
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>182</v>
@@ -3210,7 +3167,7 @@
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>183</v>
@@ -3236,7 +3193,7 @@
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>184</v>
@@ -3262,7 +3219,7 @@
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>185</v>
@@ -3288,7 +3245,7 @@
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>186</v>
@@ -3314,7 +3271,7 @@
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>187</v>
@@ -3340,10 +3297,10 @@
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
@@ -3366,7 +3323,7 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>188</v>
@@ -3392,7 +3349,7 @@
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>189</v>
@@ -3401,24 +3358,24 @@
         <v>8</v>
       </c>
       <c r="E19" s="10">
-        <v>2.3966446974236066E-3</v>
+        <v>1.1983223487118033E-3</v>
       </c>
       <c r="F19" s="10">
-        <v>2.3966446974236066E-3</v>
+        <v>1.1983223487118033E-3</v>
       </c>
       <c r="G19" s="10">
-        <v>2.3966446974236066E-3</v>
+        <v>1.1983223487118033E-3</v>
       </c>
       <c r="H19" s="10">
-        <v>2.3966446974236066E-3</v>
+        <v>1.1983223487118033E-3</v>
       </c>
       <c r="I19" s="10">
-        <v>2.3966446974236066E-3</v>
+        <v>1.1983223487118033E-3</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>190</v>
@@ -3444,7 +3401,7 @@
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>191</v>
@@ -3470,7 +3427,7 @@
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>192</v>
@@ -3478,53 +3435,26 @@
       <c r="D22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="10">
-        <v>1.1983223487118033E-3</v>
-      </c>
-      <c r="F22" s="10">
-        <v>1.1983223487118033E-3</v>
-      </c>
-      <c r="G22" s="10">
-        <v>1.1983223487118033E-3</v>
-      </c>
-      <c r="H22" s="10">
-        <v>1.1983223487118033E-3</v>
-      </c>
-      <c r="I22" s="10">
-        <v>1.1983223487118033E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="4">
-        <f>1-SUM(E3:E22)</f>
-        <v>5.9916117435609983E-4</v>
-      </c>
-      <c r="F23" s="4">
-        <v>5.9916117435590164E-4</v>
-      </c>
-      <c r="G23" s="4">
-        <v>5.9916117435590164E-4</v>
-      </c>
-      <c r="H23" s="4">
-        <v>5.9916117435590164E-4</v>
-      </c>
-      <c r="I23" s="4">
-        <v>5.9916117435590164E-4</v>
+      <c r="E22" s="19">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="F22" s="19">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="G22" s="19">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="H22" s="19">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="I22" s="19">
+        <v>5.9999999999999995E-4</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="8qHOytlnKTHRJ4G6gMQQmOascjRAj6A4UAcX/KjRNm7TDWoYhMoiKw6bPJokfwF5FoQ+cAKEge4TSK0ZYewRvw==" saltValue="RRot3/6BESi78u85WDF4UQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="wggCD/KesDnlRkftHyYWShU3uIKz9q35oXbjAkJ37exthFWWLCiwS1AJhmgIL1L+0H+B8evwQ1ByyFadVZuwWw==" saltValue="giE1X+PAw9mS/y+NNDv5nQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:I23" xr:uid="{5F25A177-8CF3-40BB-8ABD-0AE9CE8F34E1}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:I22" xr:uid="{5F25A177-8CF3-40BB-8ABD-0AE9CE8F34E1}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -4175,10 +4105,10 @@
   <sheetPr codeName="Sheet16">
     <tabColor rgb="FFFFF2CC"/>
   </sheetPr>
-  <dimension ref="B2:I23"/>
+  <dimension ref="B2:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4216,10 +4146,10 @@
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -4242,7 +4172,7 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>175</v>
@@ -4268,7 +4198,7 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>176</v>
@@ -4294,7 +4224,7 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>177</v>
@@ -4320,7 +4250,7 @@
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>178</v>
@@ -4346,7 +4276,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>179</v>
@@ -4372,7 +4302,7 @@
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>180</v>
@@ -4398,7 +4328,7 @@
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>181</v>
@@ -4424,7 +4354,7 @@
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>182</v>
@@ -4450,7 +4380,7 @@
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>183</v>
@@ -4476,7 +4406,7 @@
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>184</v>
@@ -4502,7 +4432,7 @@
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>185</v>
@@ -4528,7 +4458,7 @@
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>186</v>
@@ -4554,7 +4484,7 @@
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>187</v>
@@ -4580,10 +4510,10 @@
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
@@ -4606,7 +4536,7 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>188</v>
@@ -4632,7 +4562,7 @@
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>189</v>
@@ -4641,24 +4571,24 @@
         <v>8</v>
       </c>
       <c r="E19" s="10">
-        <v>2.3966446974236066E-3</v>
+        <v>1.1983223487118033E-3</v>
       </c>
       <c r="F19" s="10">
-        <v>2.3966446974236066E-3</v>
+        <v>1.1983223487118033E-3</v>
       </c>
       <c r="G19" s="10">
-        <v>2.3966446974236066E-3</v>
+        <v>1.1983223487118033E-3</v>
       </c>
       <c r="H19" s="10">
-        <v>2.3966446974236066E-3</v>
+        <v>1.1983223487118033E-3</v>
       </c>
       <c r="I19" s="10">
-        <v>2.3966446974236066E-3</v>
+        <v>1.1983223487118033E-3</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>190</v>
@@ -4684,7 +4614,7 @@
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>191</v>
@@ -4710,7 +4640,7 @@
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>192</v>
@@ -4718,53 +4648,26 @@
       <c r="D22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="10">
-        <v>1.1983223487118033E-3</v>
-      </c>
-      <c r="F22" s="10">
-        <v>1.1983223487118033E-3</v>
-      </c>
-      <c r="G22" s="10">
-        <v>1.1983223487118033E-3</v>
-      </c>
-      <c r="H22" s="10">
-        <v>1.1983223487118033E-3</v>
-      </c>
-      <c r="I22" s="10">
-        <v>1.1983223487118033E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="4">
-        <f>1-SUM(E3:E22)</f>
-        <v>5.9916117435609983E-4</v>
-      </c>
-      <c r="F23" s="4">
-        <v>5.9916117435590164E-4</v>
-      </c>
-      <c r="G23" s="4">
-        <v>5.9916117435590164E-4</v>
-      </c>
-      <c r="H23" s="4">
-        <v>5.9916117435590164E-4</v>
-      </c>
-      <c r="I23" s="4">
-        <v>5.9916117435590164E-4</v>
+      <c r="E22" s="19">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="F22" s="19">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="G22" s="19">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="H22" s="19">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="I22" s="19">
+        <v>5.9999999999999995E-4</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="9PrNslaL0ga7DJzGBLb/ITwYZah8w4dPzZA/iEsSUBtRnah55JJ2Wu0+C7FFK3zj/cUnC0HstEMmtWkiP40QHA==" saltValue="fUb4o9KWIASSDd7dsD6GAw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="akCQdXJzScnRvD1qF4nBDBIfJXNFqXpJWheZUonjx49WyZLyXVSSSYZMOjsIlDKej4k2XUS9Hf/x7xYawnCXKQ==" saltValue="+mfVwwYSLDCYzw2YcWX9QA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:I23" xr:uid="{4587F331-C10C-4C2C-9D6A-8C994FCBF1F2}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:I22" xr:uid="{4587F331-C10C-4C2C-9D6A-8C994FCBF1F2}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -4892,7 +4795,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -5918,10 +5821,10 @@
   <sheetPr codeName="Sheet7">
     <tabColor rgb="FFFFF2CC"/>
   </sheetPr>
-  <dimension ref="B2:I23"/>
+  <dimension ref="B2:I22"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5959,10 +5862,10 @@
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -5985,7 +5888,7 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>175</v>
@@ -6011,7 +5914,7 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>176</v>
@@ -6037,7 +5940,7 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>177</v>
@@ -6063,7 +5966,7 @@
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>178</v>
@@ -6089,7 +5992,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>179</v>
@@ -6115,7 +6018,7 @@
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>180</v>
@@ -6141,7 +6044,7 @@
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>181</v>
@@ -6167,7 +6070,7 @@
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>182</v>
@@ -6193,7 +6096,7 @@
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>183</v>
@@ -6219,7 +6122,7 @@
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>184</v>
@@ -6245,7 +6148,7 @@
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>185</v>
@@ -6271,7 +6174,7 @@
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>186</v>
@@ -6297,7 +6200,7 @@
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>187</v>
@@ -6323,10 +6226,10 @@
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
@@ -6349,7 +6252,7 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>188</v>
@@ -6375,7 +6278,7 @@
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>189</v>
@@ -6384,24 +6287,24 @@
         <v>8</v>
       </c>
       <c r="E19" s="10">
-        <v>2.3966446974236066E-3</v>
+        <v>1.1983223487118033E-3</v>
       </c>
       <c r="F19" s="10">
-        <v>2.3966446974236066E-3</v>
+        <v>1.1983223487118033E-3</v>
       </c>
       <c r="G19" s="10">
-        <v>2.3966446974236066E-3</v>
+        <v>1.1983223487118033E-3</v>
       </c>
       <c r="H19" s="10">
-        <v>2.3966446974236066E-3</v>
+        <v>1.1983223487118033E-3</v>
       </c>
       <c r="I19" s="10">
-        <v>2.3966446974236066E-3</v>
+        <v>1.1983223487118033E-3</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>190</v>
@@ -6427,7 +6330,7 @@
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>191</v>
@@ -6453,7 +6356,7 @@
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>192</v>
@@ -6461,53 +6364,26 @@
       <c r="D22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="10">
-        <v>1.1983223487118033E-3</v>
-      </c>
-      <c r="F22" s="10">
-        <v>1.1983223487118033E-3</v>
-      </c>
-      <c r="G22" s="10">
-        <v>1.1983223487118033E-3</v>
-      </c>
-      <c r="H22" s="10">
-        <v>1.1983223487118033E-3</v>
-      </c>
-      <c r="I22" s="10">
-        <v>1.1983223487118033E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="4">
-        <f>1-SUM(E3:E22)</f>
-        <v>5.9916117435609983E-4</v>
-      </c>
-      <c r="F23" s="4">
+      <c r="E22" s="19">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="F22" s="19">
         <v>5.9916117435590164E-4</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G22" s="19">
         <v>5.9916117435590164E-4</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H22" s="19">
         <v>5.9916117435590164E-4</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I22" s="19">
         <v>5.9916117435590164E-4</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="70UWWG9ULu2Yj3+aGAzp7fLzdMXp9rJnPWBsDCQNY/nkdMfIPLl0HnZ8NHLGApvMPQ0kRYfD9QiFR7I57tGNRA==" saltValue="yoKahmamOZ+jYUcmCasFSQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Ntj5NAbNesbjRFOG/7F6Yy3LSF5b1QZapNQRR1wh2n243T5qKTIkgU2Xf4JZcnxtTpqnJz5GkcJKSDewDJE++Q==" saltValue="m57K0D2hvhjiNIrQV5XZEQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:I23" xr:uid="{96703BE1-5938-4319-9C8B-21F7C46B3A7F}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:I22" xr:uid="{96703BE1-5938-4319-9C8B-21F7C46B3A7F}">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -6735,7 +6611,7 @@
   </sheetPr>
   <dimension ref="B2:I16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6876,10 +6752,10 @@
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -7118,23 +6994,23 @@
       <c r="D16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="4">
         <f>1-SUM(E9:E15)</f>
         <v>6.3000000000000056E-2</v>
       </c>
-      <c r="F16" s="20">
+      <c r="F16" s="4">
         <f t="shared" ref="F16:I16" si="0">1-SUM(F9:F15)</f>
         <v>6.3000000000000056E-2</v>
       </c>
-      <c r="G16" s="20">
+      <c r="G16" s="4">
         <f t="shared" si="0"/>
         <v>6.3000000000000056E-2</v>
       </c>
-      <c r="H16" s="20">
+      <c r="H16" s="4">
         <f t="shared" si="0"/>
         <v>6.3000000000000056E-2</v>
       </c>
-      <c r="I16" s="20">
+      <c r="I16" s="4">
         <f t="shared" si="0"/>
         <v>6.3000000000000056E-2</v>
       </c>

</xml_diff>

<commit_message>
Ensuring that tubercolosis input range is editable within assumptions sheets.
</commit_message>
<xml_diff>
--- a/data/config_inputs/lhc_config_inputs_v5.xlsx
+++ b/data/config_inputs/lhc_config_inputs_v5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csucloudservices-my.sharepoint.com/personal/elliot_royle_mlcsu_nhs_uk/Documents/Git/Lung Health Checks/data/config_inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{DEB216A3-46EC-4ECC-9D1E-00EE1BB3E5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1977D35A-792E-4C23-926B-F32D2B4F4A27}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="8_{DEB216A3-46EC-4ECC-9D1E-00EE1BB3E5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFCB9A89-588A-45A2-A40C-1BA616127717}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="29010" windowHeight="15585" firstSheet="7" activeTab="15" xr2:uid="{EEFCE178-3DE7-40FB-BEDD-2901AD1232AA}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="29010" windowHeight="15585" firstSheet="4" activeTab="6" xr2:uid="{EEFCE178-3DE7-40FB-BEDD-2901AD1232AA}"/>
   </bookViews>
   <sheets>
     <sheet name="frontpage" sheetId="1" r:id="rId1"/>
@@ -1682,7 +1682,7 @@
   <dimension ref="B2:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E22" sqref="E22:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2222,24 +2222,24 @@
       <c r="D22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="19">
+      <c r="E22" s="10">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="F22" s="19">
+      <c r="F22" s="10">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="10">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="H22" s="19">
+      <c r="H22" s="10">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="I22" s="19">
+      <c r="I22" s="10">
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="1+hkOEMOzNw0tEMYAtVoi4F9XM/W3HV3PIlcM9Oj0YjOkM++AYKe7fnVsdfMvG73GlRiyZi4JvM/tberEecYeQ==" saltValue="BmoLlpqCpN+SMl0VQ5k9RQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="M7+qidCiZ+Y8D1ZFIgoolmF4n22ofgvFF7EDfsLbucCZHolZL8oIeeyjMvjEeZi2mgRf2ygOLzhXJaW0Wecxaw==" saltValue="D5SNHtpiRRKR8ye9nIz1Tg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="1">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:I22" xr:uid="{C2D4DCCC-2F6E-43B5-9BE7-2CCD33112B93}">
       <formula1>0</formula1>
@@ -2895,7 +2895,7 @@
   <dimension ref="B2:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E22" sqref="E22:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3435,24 +3435,24 @@
       <c r="D22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="19">
+      <c r="E22" s="10">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="F22" s="19">
+      <c r="F22" s="10">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="10">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="H22" s="19">
+      <c r="H22" s="10">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="I22" s="19">
+      <c r="I22" s="10">
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="wggCD/KesDnlRkftHyYWShU3uIKz9q35oXbjAkJ37exthFWWLCiwS1AJhmgIL1L+0H+B8evwQ1ByyFadVZuwWw==" saltValue="giE1X+PAw9mS/y+NNDv5nQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="TFx2npmQudGkvCp97tN4maBdLCO/yDC32dZ4BizsIY23Q8VmJPGAxZ2y3qheKwIUCMaNXSdTB9vMIbCzXb8qzA==" saltValue="4JnT/wGIMgjAZy9Tr1TRAA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="1">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:I22" xr:uid="{5F25A177-8CF3-40BB-8ABD-0AE9CE8F34E1}">
       <formula1>0</formula1>
@@ -3683,7 +3683,7 @@
   <dimension ref="B2:I16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4107,8 +4107,8 @@
   </sheetPr>
   <dimension ref="B2:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4233,7 +4233,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="10">
-        <v>2.3966446974236066E-2</v>
+        <v>2.39664469742361E-2</v>
       </c>
       <c r="F6" s="10">
         <v>2.3966446974236066E-2</v>
@@ -4311,7 +4311,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="10">
-        <v>1.4379868184541639E-2</v>
+        <v>1.43798681845416E-2</v>
       </c>
       <c r="F9" s="10">
         <v>1.4379868184541639E-2</v>
@@ -4363,7 +4363,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="10">
-        <v>9.5865787896944263E-3</v>
+        <v>9.5865787896944298E-3</v>
       </c>
       <c r="F11" s="10">
         <v>9.5865787896944263E-3</v>
@@ -4493,7 +4493,7 @@
         <v>8</v>
       </c>
       <c r="E16" s="10">
-        <v>4.7932893948472131E-3</v>
+        <v>4.7932893948472097E-3</v>
       </c>
       <c r="F16" s="10">
         <v>4.7932893948472131E-3</v>
@@ -4600,16 +4600,16 @@
         <v>1.1983223487118033E-3</v>
       </c>
       <c r="F20" s="10">
-        <v>1.1983223487118033E-3</v>
+        <v>1.1983223487118E-3</v>
       </c>
       <c r="G20" s="10">
-        <v>1.1983223487118033E-3</v>
+        <v>1.1983223487118E-3</v>
       </c>
       <c r="H20" s="10">
         <v>1.1983223487118033E-3</v>
       </c>
       <c r="I20" s="10">
-        <v>1.1983223487118033E-3</v>
+        <v>1.1983223487118E-3</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
@@ -4623,19 +4623,19 @@
         <v>8</v>
       </c>
       <c r="E21" s="10">
-        <v>1.1983223487118033E-3</v>
+        <v>1.1983223487118E-3</v>
       </c>
       <c r="F21" s="10">
         <v>1.1983223487118033E-3</v>
       </c>
       <c r="G21" s="10">
-        <v>1.1983223487118033E-3</v>
+        <v>1.1983223487118E-3</v>
       </c>
       <c r="H21" s="10">
-        <v>1.1983223487118033E-3</v>
+        <v>1.1983223487118E-3</v>
       </c>
       <c r="I21" s="10">
-        <v>1.1983223487118033E-3</v>
+        <v>1.1983223487118E-3</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
@@ -4648,24 +4648,24 @@
       <c r="D22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="19">
+      <c r="E22" s="10">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="F22" s="19">
+      <c r="F22" s="10">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="10">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="H22" s="19">
+      <c r="H22" s="10">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="I22" s="19">
+      <c r="I22" s="10">
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="akCQdXJzScnRvD1qF4nBDBIfJXNFqXpJWheZUonjx49WyZLyXVSSSYZMOjsIlDKej4k2XUS9Hf/x7xYawnCXKQ==" saltValue="+mfVwwYSLDCYzw2YcWX9QA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="+l9nThjHTcbiVIqZsWJfY1HrJAp2OSrEwhD7ccKQUOHC0ISJPtCLC4YTB4ChtW+iXTs0Me9ClOw4H/QCzKI+XA==" saltValue="g5LAwdGcczvXKOQ+xexWZQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="1">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:I22" xr:uid="{4587F331-C10C-4C2C-9D6A-8C994FCBF1F2}">
       <formula1>0</formula1>
@@ -5823,8 +5823,8 @@
   </sheetPr>
   <dimension ref="B2:I22"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6364,24 +6364,24 @@
       <c r="D22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="19">
+      <c r="E22" s="10">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="F22" s="19">
+      <c r="F22" s="10">
         <v>5.9916117435590164E-4</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="10">
         <v>5.9916117435590164E-4</v>
       </c>
-      <c r="H22" s="19">
+      <c r="H22" s="10">
         <v>5.9916117435590164E-4</v>
       </c>
-      <c r="I22" s="19">
+      <c r="I22" s="10">
         <v>5.9916117435590164E-4</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Ntj5NAbNesbjRFOG/7F6Yy3LSF5b1QZapNQRR1wh2n243T5qKTIkgU2Xf4JZcnxtTpqnJz5GkcJKSDewDJE++Q==" saltValue="m57K0D2hvhjiNIrQV5XZEQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="xr+7nyhmSFGF/d9xfJpA6t8yVYRuCDf5JC2PN4BMiHvwiCB5kRDT5yTArWha/AxKNH1pcU6sUdt9muQZYjYNjA==" saltValue="OyrqFxIAulpTH6pgAde5Fg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="1">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:I22" xr:uid="{96703BE1-5938-4319-9C8B-21F7C46B3A7F}">
       <formula1>0</formula1>

</xml_diff>